<commit_message>
add maven and dubbo
add maven and dubbo
</commit_message>
<xml_diff>
--- a/Dubbo指南.xlsx
+++ b/Dubbo指南.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEED0A2-0854-4C00-BC38-2DD2711244F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="安装" sheetId="1" r:id="rId1"/>
@@ -15,8 +14,9 @@
     <sheet name=" " sheetId="4" r:id="rId5"/>
     <sheet name="ZooKeeper相关操作" sheetId="6" r:id="rId6"/>
     <sheet name="低配服务器的启动问题" sheetId="7" r:id="rId7"/>
+    <sheet name="Docker 搭建简单项目" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="202">
   <si>
     <t>前提条件</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -648,14 +648,22 @@
   </si>
   <si>
     <t>解决方案：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>参考文档</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://blog.csdn.net/boling_cavalry/article/details/72303126</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -668,6 +676,14 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -694,15 +710,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -729,7 +748,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{BBE6E932-C918-411D-971B-8DDDDA2E2C74}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -765,7 +784,7 @@
         <xdr:cNvPr id="2" name="图片 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECA02915-5B3A-4150-A8B1-182DCB95C1A5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ECA02915-5B3A-4150-A8B1-182DCB95C1A5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -814,7 +833,7 @@
         <xdr:cNvPr id="2" name="图片 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D6A7B94-A531-47F6-BE30-D2F7EE2153D8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5D6A7B94-A531-47F6-BE30-D2F7EE2153D8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -863,7 +882,7 @@
         <xdr:cNvPr id="3" name="图片 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A96C447-AF14-41BB-A61C-ECF3A9E8B5D7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2A96C447-AF14-41BB-A61C-ECF3A9E8B5D7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1154,21 +1173,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1181,36 +1200,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2620AF00-8098-49D8-8209-726C0E7149DA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1223,76 +1242,76 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{994ED3E7-A015-42C7-8556-3D5F83C5AC5B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="B5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="B6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="B8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="B9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="B10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="B11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="B13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="B14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="B16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:5">
       <c r="C17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:5">
       <c r="C18" t="s">
         <v>19</v>
       </c>
@@ -1300,22 +1319,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:5">
       <c r="C19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:5">
       <c r="C20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:5">
       <c r="C21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:5">
       <c r="C22" t="s">
         <v>24</v>
       </c>
@@ -1323,7 +1342,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:5">
       <c r="C23" t="s">
         <v>26</v>
       </c>
@@ -1331,7 +1350,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:5">
       <c r="C24" t="s">
         <v>28</v>
       </c>
@@ -1339,7 +1358,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:5">
       <c r="C25" t="s">
         <v>30</v>
       </c>
@@ -1347,7 +1366,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:5">
       <c r="C26" t="s">
         <v>32</v>
       </c>
@@ -1355,7 +1374,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:5">
       <c r="C27" t="s">
         <v>34</v>
       </c>
@@ -1363,7 +1382,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:5">
       <c r="C28" t="s">
         <v>36</v>
       </c>
@@ -1371,157 +1390,157 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:5">
       <c r="C29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:5">
       <c r="C30" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:5">
       <c r="C31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:5">
       <c r="C32" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:5">
       <c r="C33" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5">
       <c r="C34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5">
       <c r="C35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:5">
       <c r="C36" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5">
       <c r="C37" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:5">
       <c r="B38" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:5">
       <c r="B40" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:5">
       <c r="B41" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:5">
       <c r="C42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:5">
       <c r="C43" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:5">
       <c r="D44" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:5">
       <c r="E45" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:5">
       <c r="E46" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:5">
       <c r="E47" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:5">
       <c r="E48" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:8">
       <c r="F49" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:8">
       <c r="E50" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:8">
       <c r="E51" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:8">
       <c r="F52" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:8">
       <c r="G53" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:8">
       <c r="G54" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:8">
       <c r="H55" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:8">
       <c r="G56" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:8">
       <c r="F57" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="4:8">
       <c r="E58" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="4:8">
       <c r="D59" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="4:8">
       <c r="D61" t="s">
         <v>52</v>
       </c>
@@ -1529,82 +1548,82 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="4:8">
       <c r="E62" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="4:8">
       <c r="E63" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="4:8">
       <c r="E64" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6">
       <c r="E65" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6">
       <c r="F66" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6">
       <c r="F67" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6">
       <c r="F68" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6">
       <c r="E69" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6">
       <c r="D70" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6">
       <c r="C71" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6">
       <c r="B72" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1">
       <c r="A83" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1">
       <c r="A84" t="s">
         <v>80</v>
       </c>
@@ -1616,126 +1635,126 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C770187-0C4A-4F3E-835E-0A372317D815}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H242"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A109" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="B5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="B6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="B8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="B9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="C10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="C11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="C12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="C13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="B14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4">
       <c r="B17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4">
       <c r="B18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4">
       <c r="B19" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4">
       <c r="B20" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4">
       <c r="B21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4">
       <c r="B23" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4">
       <c r="B24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:4">
       <c r="C25" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4">
       <c r="C26" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:4">
       <c r="B27" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:4">
       <c r="B29" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:4">
       <c r="C30" t="s">
         <v>97</v>
       </c>
@@ -1743,27 +1762,27 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:4">
       <c r="D31" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:4">
       <c r="D32" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:6">
       <c r="D33" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:6">
       <c r="C34" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:6">
       <c r="C35" t="s">
         <v>97</v>
       </c>
@@ -1771,57 +1790,57 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:6">
       <c r="D36" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:6">
       <c r="D37" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:6">
       <c r="D38" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:6">
       <c r="D39" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:6">
       <c r="E40" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:6">
       <c r="F41" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:6">
       <c r="F42" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:6">
       <c r="E43" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:6">
       <c r="D44" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:6">
       <c r="C45" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:6">
       <c r="C46" t="s">
         <v>97</v>
       </c>
@@ -1829,792 +1848,792 @@
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:6">
       <c r="D47" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:6">
       <c r="D48" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:6">
       <c r="D49" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:6">
       <c r="D50" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:6">
       <c r="E51" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:6">
       <c r="F52" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:6">
       <c r="F53" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:6">
       <c r="E54" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:6">
       <c r="E55" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:6">
       <c r="F56" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:6">
       <c r="F57" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:6">
       <c r="E58" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:6">
       <c r="E59" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:6">
       <c r="F60" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="61" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:6">
       <c r="F61" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:6">
       <c r="E62" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="63" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:6">
       <c r="D63" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="64" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:6">
       <c r="C64" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:6">
       <c r="C65" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:6">
       <c r="D66" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:6">
       <c r="D67" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:6">
       <c r="D68" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:6">
       <c r="D69" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:6">
       <c r="E70" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:6">
       <c r="F71" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:6">
       <c r="F72" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:6">
       <c r="E73" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:6">
       <c r="D74" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="75" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:6">
       <c r="C75" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="76" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="3:6">
       <c r="C76" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:6">
       <c r="C77" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="78" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="3:6">
       <c r="D78" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="79" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="3:6">
       <c r="D79" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="80" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="3:6">
       <c r="D80" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="81" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="3:6">
       <c r="C81" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="3:6">
       <c r="C82" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="83" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="3:6">
       <c r="D83" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="3:6">
       <c r="D84" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="85" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="3:6">
       <c r="D85" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="3:6">
       <c r="C86" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="3:6">
       <c r="C87" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="88" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="3:6">
       <c r="D88" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="89" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="3:6">
       <c r="D89" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="90" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="3:6">
       <c r="D90" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="91" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="3:6">
       <c r="D91" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="92" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="3:6">
       <c r="E92" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="93" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="3:6">
       <c r="F93" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="94" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="3:6">
       <c r="F94" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="95" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="3:6">
       <c r="E95" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="96" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="3:6">
       <c r="D96" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="97" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="3:6">
       <c r="C97" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="3:6">
       <c r="C98" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="3:6">
       <c r="D99" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="100" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="3:6">
       <c r="D100" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="101" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="3:6">
       <c r="D101" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="102" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="3:6">
       <c r="C102" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="3:6">
       <c r="C103" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="104" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="3:6">
       <c r="D104" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="105" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="3:6">
       <c r="D105" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="106" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="3:6">
       <c r="D106" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="107" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="3:6">
       <c r="D107" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="3:6">
       <c r="E108" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="3:6">
       <c r="F109" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="110" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="3:6">
       <c r="F110" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="111" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="3:6">
       <c r="E111" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="3:6">
       <c r="D112" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="3:4">
       <c r="C113" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="114" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="3:4">
       <c r="C114" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="3:4">
       <c r="C115" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="116" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="3:4">
       <c r="D116" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="117" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="3:4">
       <c r="D117" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="118" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="3:4">
       <c r="D118" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="119" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="3:4">
       <c r="C119" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="120" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="3:4">
       <c r="C120" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="121" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="3:4">
       <c r="D121" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="122" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="3:4">
       <c r="D122" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="123" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="3:4">
       <c r="D123" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="124" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="3:4">
       <c r="C124" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="125" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="3:4">
       <c r="C125" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="126" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="3:4">
       <c r="D126" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="127" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="3:4">
       <c r="D127" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="128" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="3:4">
       <c r="D128" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="129" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="3:4">
       <c r="C129" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="130" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="3:4">
       <c r="C130" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="131" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="3:4">
       <c r="D131" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="132" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="3:4">
       <c r="D132" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="133" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="3:4">
       <c r="D133" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="134" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="3:4">
       <c r="C134" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="135" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="3:4">
       <c r="C135" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="136" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="3:4">
       <c r="C136" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="137" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="3:4">
       <c r="D137" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="138" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="3:4">
       <c r="D138" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="139" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="3:4">
       <c r="D139" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="140" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="3:4">
       <c r="C140" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="141" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="3:4">
       <c r="C141" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="142" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="3:4">
       <c r="D142" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="143" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="3:4">
       <c r="D143" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="144" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="3:4">
       <c r="D144" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="145" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="3:4">
       <c r="C145" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="146" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="3:4">
       <c r="C146" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="147" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="3:4">
       <c r="D147" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="148" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="3:4">
       <c r="D148" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="149" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="3:4">
       <c r="D149" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="150" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="3:4">
       <c r="C150" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="151" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="3:4">
       <c r="C151" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="152" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="3:4">
       <c r="D152" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="153" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="3:4">
       <c r="D153" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="154" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="3:4">
       <c r="D154" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="155" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="3:4">
       <c r="C155" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="156" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="3:4">
       <c r="C156" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="157" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="3:4">
       <c r="D157" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="158" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="3:4">
       <c r="D158" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="159" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="3:4">
       <c r="D159" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="160" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="160" spans="3:4">
       <c r="C160" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="161" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:5">
       <c r="C161" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="162" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:5">
       <c r="D162" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="163" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:5">
       <c r="D163" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="164" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:5">
       <c r="D164" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="165" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:5">
       <c r="C165" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="166" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:5">
       <c r="B166" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="168" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:5">
       <c r="B168" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="169" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:5">
       <c r="B169" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="170" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:5">
       <c r="C170" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="171" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:5">
       <c r="D171" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="172" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:5">
       <c r="D172" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:5">
       <c r="E173" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="174" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:5">
       <c r="D174" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="175" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:5">
       <c r="D175" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="176" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:5">
       <c r="E176" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="177" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="177" spans="3:5">
       <c r="D177" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="178" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="3:5">
       <c r="C178" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="179" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="3:5">
       <c r="C179" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="180" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="3:5">
       <c r="D180" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="181" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="181" spans="3:5">
       <c r="D181" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="182" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="3:5">
       <c r="E182" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="183" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="3:5">
       <c r="D183" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="184" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="3:5">
       <c r="D184" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="185" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="185" spans="3:5">
       <c r="E185" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="186" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="186" spans="3:5">
       <c r="D186" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="187" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="187" spans="3:5">
       <c r="C187" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="188" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="188" spans="3:5">
       <c r="C188" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="189" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="189" spans="3:5">
       <c r="D189" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="190" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="190" spans="3:5">
       <c r="D190" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="191" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="191" spans="3:5">
       <c r="E191" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="192" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="192" spans="3:5">
       <c r="D192" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="193" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:5">
       <c r="D193" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="194" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:5">
       <c r="E194" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="195" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:5">
       <c r="D195" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="196" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:5">
       <c r="C196" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="197" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:5">
       <c r="B197" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="199" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:5">
       <c r="B199" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="200" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:5">
       <c r="C200" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="201" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:5">
       <c r="C201" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="202" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:5">
       <c r="D202" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="203" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:5">
       <c r="E203" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="204" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:5">
       <c r="E204" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="205" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:5">
       <c r="D205" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="206" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:5">
       <c r="D206" t="s">
         <v>174</v>
       </c>
@@ -2622,182 +2641,182 @@
         <v>175</v>
       </c>
     </row>
-    <row r="207" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:5">
       <c r="E207" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="208" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:5">
       <c r="E208" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="209" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="209" spans="3:7">
       <c r="D209" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="210" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="210" spans="3:7">
       <c r="C210" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="211" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="211" spans="3:7">
       <c r="C211" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="212" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="212" spans="3:7">
       <c r="D212" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="213" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="213" spans="3:7">
       <c r="E213" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="214" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="214" spans="3:7">
       <c r="E214" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="215" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="215" spans="3:7">
       <c r="E215" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="216" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="216" spans="3:7">
       <c r="E216" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="217" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="217" spans="3:7">
       <c r="F217" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="218" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="218" spans="3:7">
       <c r="F218" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="219" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="219" spans="3:7">
       <c r="G219" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="220" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="220" spans="3:7">
       <c r="G220" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="221" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="221" spans="3:7">
       <c r="G221" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="222" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="222" spans="3:7">
       <c r="F222" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="223" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="223" spans="3:7">
       <c r="E223" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="224" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="224" spans="3:7">
       <c r="D224" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="225" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="225" spans="3:8">
       <c r="D225" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="226" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="226" spans="3:8">
       <c r="E226" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="227" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="227" spans="3:8">
       <c r="E227" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="228" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="228" spans="3:8">
       <c r="F228" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="229" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="229" spans="3:8">
       <c r="E229" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="230" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="230" spans="3:8">
       <c r="E230" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="231" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="231" spans="3:8">
       <c r="F231" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="232" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="232" spans="3:8">
       <c r="G232" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="233" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="233" spans="3:8">
       <c r="G233" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="234" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="234" spans="3:8">
       <c r="G234" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="235" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="235" spans="3:8">
       <c r="H235" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="236" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="236" spans="3:8">
       <c r="G236" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="237" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="237" spans="3:8">
       <c r="F237" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="238" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="238" spans="3:8">
       <c r="E238" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="239" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="239" spans="3:8">
       <c r="D239" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="240" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="240" spans="3:8">
       <c r="C240" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:2">
       <c r="B241" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:2">
       <c r="A242" t="s">
         <v>74</v>
       </c>
@@ -2809,96 +2828,96 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{757D9135-7409-4C08-B2A0-679114B4AA5D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="B4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="B5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="B7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="B8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="C9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="C10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="C11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="B12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="B14" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="B15" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="B16" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="B17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -2910,36 +2929,36 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D0A7B3-3664-4CDE-9CDF-5D7E135ACE8F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>194</v>
       </c>
@@ -2952,36 +2971,36 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCE5053-1EAA-4A72-8CD4-004179BE8FC2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>195</v>
       </c>
@@ -2992,4 +3011,33 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>